<commit_message>
start conference on May 18 as a test on excel file, bug fix
</commit_message>
<xml_diff>
--- a/pm2024/pm2024.xlsx
+++ b/pm2024/pm2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galli/Documents/OrgConferenze/24PisaMeeting/pisameet/pm2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C487AA74-C628-8641-AA3B-2B7D9C31F4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D71C63-80C7-2549-997F-B7C000E29059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="27260" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="1022">
   <si>
     <t>Session ID</t>
   </si>
@@ -3097,6 +3097,9 @@
   </si>
   <si>
     <t>Kyung Hee University</t>
+  </si>
+  <si>
+    <t>18/05/2024 08:00</t>
   </si>
 </sst>
 </file>
@@ -3160,7 +3163,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3498,7 +3501,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3529,8 +3532,8 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
-        <v>45430.333333333336</v>
+      <c r="C2" s="2" t="s">
+        <v>1021</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -3543,8 +3546,8 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>45430.333333333336</v>
+      <c r="C3" s="2" t="s">
+        <v>1021</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>

</xml_diff>